<commit_message>
Something is broken. I get this error: [1] "Sim: 1 of 5" Error in if (pred_catch < catch) { :   missing value where TRUE/FALSE needed
</commit_message>
<xml_diff>
--- a/data/catch_input_conditioning.xlsx
+++ b/data/catch_input_conditioning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14610" windowHeight="14490" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="14610" windowHeight="14490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6395,9 +6395,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6444,7 +6446,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -6485,7 +6487,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
@@ -6526,7 +6528,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -6567,7 +6569,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -6608,7 +6610,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
@@ -6649,7 +6651,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
@@ -6690,7 +6692,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
@@ -6731,7 +6733,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
@@ -6772,7 +6774,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
@@ -6813,7 +6815,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
@@ -6854,7 +6856,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
@@ -6895,7 +6897,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -6936,7 +6938,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
@@ -6977,7 +6979,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B15" s="6">
         <v>1</v>
@@ -7018,7 +7020,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B16" s="6">
         <v>1</v>
@@ -7059,7 +7061,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B17" s="6">
         <v>1</v>
@@ -7100,7 +7102,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B18" s="6">
         <v>1</v>
@@ -7141,7 +7143,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
@@ -7182,7 +7184,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
@@ -7223,7 +7225,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -7264,7 +7266,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
@@ -7305,7 +7307,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B23" s="6">
         <v>1</v>
@@ -7346,7 +7348,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B24" s="6">
         <v>1</v>
@@ -7387,7 +7389,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B25" s="6">
         <v>1</v>
@@ -7428,7 +7430,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B26" s="6">
         <v>1</v>
@@ -7469,7 +7471,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B27" s="6">
         <v>1</v>
@@ -7510,7 +7512,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B28" s="6">
         <v>1</v>
@@ -7551,7 +7553,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B29" s="6">
         <v>1</v>
@@ -7592,7 +7594,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
@@ -7633,7 +7635,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B31" s="6">
         <v>1</v>
@@ -7674,7 +7676,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B32" s="6">
         <v>1</v>
@@ -7715,7 +7717,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B33" s="6">
         <v>1</v>
@@ -7756,7 +7758,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B34" s="6">
         <v>1</v>
@@ -7797,7 +7799,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B35" s="6">
         <v>1</v>
@@ -7838,7 +7840,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B36" s="6">
         <v>1</v>
@@ -7879,7 +7881,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B37" s="6">
         <v>1</v>
@@ -7920,7 +7922,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B38" s="6">
         <v>1</v>
@@ -7961,7 +7963,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B39" s="6">
         <v>1</v>
@@ -8002,7 +8004,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B40" s="6">
         <v>1</v>
@@ -8043,7 +8045,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B41" s="6">
         <v>1</v>
@@ -8084,7 +8086,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B42" s="6">
         <v>1</v>
@@ -8125,7 +8127,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B43" s="6">
         <v>1</v>
@@ -8161,6 +8163,47 @@
         <v>4</v>
       </c>
       <c r="M43" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2018</v>
+      </c>
+      <c r="B44" s="6">
+        <v>1</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="D44" s="6">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F44" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="H44" s="6">
+        <v>5</v>
+      </c>
+      <c r="I44" s="6">
+        <v>1</v>
+      </c>
+      <c r="J44" s="6">
+        <v>2</v>
+      </c>
+      <c r="K44" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="L44" s="6">
+        <v>4</v>
+      </c>
+      <c r="M44" s="6">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>